<commit_message>
Volt Var debugging complete
</commit_message>
<xml_diff>
--- a/ProjectFiles/HECO/PyDSS Settings/HP-VV-VW-A/pyPlotList/Time series.xlsx
+++ b/ProjectFiles/HECO/PyDSS Settings/HP-VV-VW-A/pyPlotList/Time series.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19001"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Controllers" sheetId="1" r:id="rId1"/>
@@ -89,27 +89,18 @@
     <t>TS2</t>
   </si>
   <si>
-    <t>['Index=0']</t>
-  </si>
-  <si>
     <t>ObjectType</t>
   </si>
   <si>
     <t>Circuit</t>
   </si>
   <si>
-    <t>PVSystem.oh_263163_0_1</t>
-  </si>
-  <si>
     <t>nSamples</t>
   </si>
   <si>
     <t>Dynamic</t>
   </si>
   <si>
-    <t>dev_263265_0_1</t>
-  </si>
-  <si>
     <t>['v.Powers','v.Powers']</t>
   </si>
   <si>
@@ -117,6 +108,15 @@
   </si>
   <si>
     <t>['SumEven','SumOdd']</t>
+  </si>
+  <si>
+    <t>PVSystem.oh_261584_2_4</t>
+  </si>
+  <si>
+    <t>dev_261585_2_4</t>
+  </si>
+  <si>
+    <t>['Even']</t>
   </si>
 </sst>
 </file>
@@ -912,23 +912,23 @@
   <dimension ref="A1:J28"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="75.5546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="55.88671875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="75.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="55.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.42578125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="13" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.5546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="18" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B1" s="1"/>
       <c r="C1" s="9"/>
       <c r="D1" s="10"/>
@@ -937,7 +937,7 @@
       <c r="G1" s="18"/>
       <c r="H1" s="18"/>
     </row>
-    <row r="2" spans="1:10" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:10" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="12" t="s">
         <v>16</v>
       </c>
@@ -963,30 +963,30 @@
         <v>14</v>
       </c>
       <c r="I2" s="17" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="J2" s="17" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
         <v>20</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="C3" s="11" t="s">
         <v>15</v>
       </c>
       <c r="D3" s="11" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="E3" s="11" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="F3" s="11" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="G3" s="11">
         <v>1400</v>
@@ -1001,12 +1001,12 @@
         <v>96</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
         <v>21</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C4" s="11" t="s">
         <v>19</v>
@@ -1018,7 +1018,7 @@
         <v>17</v>
       </c>
       <c r="F4" s="11" t="s">
-        <v>22</v>
+        <v>31</v>
       </c>
       <c r="G4" s="11">
         <v>1400</v>
@@ -1033,7 +1033,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B5" s="7"/>
       <c r="C5" s="7"/>
       <c r="D5" s="7"/>
@@ -1042,7 +1042,7 @@
       <c r="G5" s="7"/>
       <c r="H5" s="7"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B6" s="7"/>
       <c r="C6" s="7"/>
       <c r="D6" s="7"/>
@@ -1051,7 +1051,7 @@
       <c r="G6" s="7"/>
       <c r="H6" s="7"/>
     </row>
-    <row r="7" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="7"/>
       <c r="C7" s="7"/>
       <c r="D7" s="7"/>
@@ -1060,7 +1060,7 @@
       <c r="G7" s="7"/>
       <c r="H7" s="7"/>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B8" s="7"/>
       <c r="C8" s="7"/>
       <c r="D8" s="7"/>
@@ -1069,7 +1069,7 @@
       <c r="G8" s="7"/>
       <c r="H8" s="7"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B9" s="7"/>
       <c r="C9" s="7"/>
       <c r="D9" s="7"/>
@@ -1078,7 +1078,7 @@
       <c r="G9" s="7"/>
       <c r="H9" s="7"/>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B10" s="7"/>
       <c r="C10" s="7"/>
       <c r="D10" s="7"/>
@@ -1087,7 +1087,7 @@
       <c r="G10" s="7"/>
       <c r="H10" s="7"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B11" s="7"/>
       <c r="C11" s="7"/>
       <c r="D11" s="7"/>
@@ -1096,7 +1096,7 @@
       <c r="G11" s="7"/>
       <c r="H11" s="7"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B12" s="7"/>
       <c r="C12" s="7"/>
       <c r="D12" s="7"/>
@@ -1105,7 +1105,7 @@
       <c r="G12" s="7"/>
       <c r="H12" s="7"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B13" s="7"/>
       <c r="C13" s="7"/>
       <c r="D13" s="7"/>
@@ -1114,7 +1114,7 @@
       <c r="G13" s="7"/>
       <c r="H13" s="7"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B14" s="7"/>
       <c r="C14" s="7"/>
       <c r="D14" s="7"/>
@@ -1123,7 +1123,7 @@
       <c r="G14" s="7"/>
       <c r="H14" s="7"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B15" s="7"/>
       <c r="C15" s="7"/>
       <c r="D15" s="7"/>
@@ -1132,7 +1132,7 @@
       <c r="G15" s="7"/>
       <c r="H15" s="7"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B16" s="7"/>
       <c r="C16" s="7"/>
       <c r="D16" s="7"/>
@@ -1141,7 +1141,7 @@
       <c r="G16" s="7"/>
       <c r="H16" s="7"/>
     </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B17" s="7"/>
       <c r="C17" s="7"/>
       <c r="D17" s="7"/>
@@ -1150,7 +1150,7 @@
       <c r="G17" s="7"/>
       <c r="H17" s="7"/>
     </row>
-    <row r="18" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B18" s="7"/>
       <c r="C18" s="7"/>
       <c r="D18" s="7"/>
@@ -1159,7 +1159,7 @@
       <c r="G18" s="7"/>
       <c r="H18" s="7"/>
     </row>
-    <row r="19" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B19" s="7"/>
       <c r="C19" s="7"/>
       <c r="D19" s="7"/>
@@ -1168,7 +1168,7 @@
       <c r="G19" s="7"/>
       <c r="H19" s="7"/>
     </row>
-    <row r="20" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B20" s="7"/>
       <c r="C20" s="7"/>
       <c r="D20" s="7"/>
@@ -1177,7 +1177,7 @@
       <c r="G20" s="7"/>
       <c r="H20" s="7"/>
     </row>
-    <row r="21" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B21" s="7"/>
       <c r="C21" s="7"/>
       <c r="D21" s="7"/>
@@ -1186,7 +1186,7 @@
       <c r="G21" s="7"/>
       <c r="H21" s="7"/>
     </row>
-    <row r="22" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B22" s="7"/>
       <c r="C22" s="7"/>
       <c r="D22" s="7"/>
@@ -1195,7 +1195,7 @@
       <c r="G22" s="7"/>
       <c r="H22" s="7"/>
     </row>
-    <row r="23" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B23" s="7"/>
       <c r="C23" s="7"/>
       <c r="D23" s="7"/>
@@ -1204,7 +1204,7 @@
       <c r="G23" s="7"/>
       <c r="H23" s="7"/>
     </row>
-    <row r="24" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B24" s="7"/>
       <c r="C24" s="7"/>
       <c r="D24" s="7"/>
@@ -1213,7 +1213,7 @@
       <c r="G24" s="7"/>
       <c r="H24" s="7"/>
     </row>
-    <row r="25" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B25" s="7"/>
       <c r="C25" s="7"/>
       <c r="D25" s="7"/>
@@ -1222,7 +1222,7 @@
       <c r="G25" s="7"/>
       <c r="H25" s="7"/>
     </row>
-    <row r="26" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B26" s="7"/>
       <c r="C26" s="7"/>
       <c r="D26" s="7"/>
@@ -1231,7 +1231,7 @@
       <c r="G26" s="7"/>
       <c r="H26" s="7"/>
     </row>
-    <row r="27" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B27" s="7"/>
       <c r="C27" s="7"/>
       <c r="D27" s="7"/>
@@ -1240,7 +1240,7 @@
       <c r="G27" s="7"/>
       <c r="H27" s="7"/>
     </row>
-    <row r="28" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B28" s="7"/>
       <c r="C28" s="7"/>
       <c r="D28" s="7"/>
@@ -1281,20 +1281,20 @@
       <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.88671875" customWidth="1"/>
-    <col min="2" max="2" width="15.44140625" customWidth="1"/>
-    <col min="3" max="3" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.85546875" customWidth="1"/>
+    <col min="2" max="2" width="15.42578125" customWidth="1"/>
+    <col min="3" max="3" width="17.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="21" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:3" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="19" t="s">
         <v>7</v>
       </c>
       <c r="B1" s="19"/>
     </row>
-    <row r="2" spans="1:3" ht="18" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
@@ -1302,10 +1302,10 @@
         <v>1</v>
       </c>
       <c r="C2" s="16" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>4</v>
       </c>
@@ -1316,7 +1316,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>5</v>
       </c>
@@ -1327,16 +1327,16 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>2</v>
       </c>
       <c r="B5" s="2"/>
       <c r="C5" s="15" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>3</v>
       </c>

</xml_diff>